<commit_message>
chore: template reconsiliasi update validasi akun di template csv
</commit_message>
<xml_diff>
--- a/assets/templates/rekonsiliasi.xlsx
+++ b/assets/templates/rekonsiliasi.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Klien\LC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/workspace/repo/node-repo/lc-project/packages/lc-webapp/assets/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34174DC-41C2-324E-9F1E-197E60772B77}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21333" windowHeight="8400"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21340" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template-reconciliation" sheetId="1" r:id="rId1"/>
     <sheet name="AKUN" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="218">
   <si>
     <t>Laporan Kas BCA  Bulan FEBRUARI 2021</t>
   </si>
@@ -671,12 +672,15 @@
   </si>
   <si>
     <t>PAJAK BUNGA</t>
+  </si>
+  <si>
+    <t>Kode Akun Bank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1479,27 +1483,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.9375" customWidth="1"/>
-    <col min="2" max="2" width="8.9375" customWidth="1"/>
-    <col min="6" max="6" width="12.3515625" customWidth="1"/>
-    <col min="7" max="7" width="32.17578125" customWidth="1"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="F1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G1">
+        <v>1010305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1522,7 +1532,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44243</v>
       </c>
@@ -1543,7 +1553,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44246</v>
       </c>
@@ -1564,7 +1574,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44255</v>
       </c>
@@ -1585,7 +1595,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44255</v>
       </c>
@@ -1606,457 +1616,457 @@
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F7" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G7,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F8" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G8,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F9" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G9,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F10" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G10,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F11" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G11,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F12" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G12,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F13" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G13,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F14" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G14,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F15" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G15,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F16" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G16,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G17,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F18" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G18,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G19,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F20" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G20,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F21" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G21,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F22" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G22,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="23" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F23" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G23,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F24" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G24,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="25" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F25" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G25,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="26" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F26" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G26,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="27" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F27" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G27,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="28" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F28" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G28,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="29" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F29" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G29,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="30" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F30" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G30,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="31" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F31" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G31,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="32" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F32" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G32,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F33" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G33,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F34" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G34,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="35" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F35" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G35,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="36" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F36" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G36,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="37" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F37" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G37,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="38" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F38" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G38,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="39" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F39" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G39,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="40" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F40" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G40,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="41" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F41" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G41,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="42" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F42" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G42,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="43" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F43" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G43,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="44" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F44" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G44,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="45" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F45" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G45,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="46" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F46" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G46,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="47" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="47" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F47" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G47,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="48" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="48" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F48" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G48,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F49" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G49,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="50" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G50,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="51" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F51" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G51,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="52" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F52" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G52,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="53" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F53" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G53,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="54" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F54" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G54,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="55" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F55" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G55,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="56" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F56" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G56,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="57" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F57" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G57,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="58" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F58" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G58,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="59" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F59" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G59,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="60" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F60" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G60,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="61" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F61" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G61,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="62" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="62" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F62" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G62,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="63" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="63" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F63" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G63,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="64" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="64" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F64" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G64,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="65" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F65" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G65,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="66" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F66" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G66,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="67" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F67" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G67,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="68" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F68" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G68,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="69" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F69" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G69,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="70" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F70" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G70,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="71" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F71" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G71,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="72" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F72" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G72,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="73" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F73" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G73,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="74" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F74" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G74,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="75" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F75" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G75,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="76" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F76" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G76,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="77" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="77" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F77" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G77,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="78" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="78" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F78" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G78,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="79" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="79" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F79" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G79,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="80" spans="6:6" x14ac:dyDescent="0.5">
+    <row r="80" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F80" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G80,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F81" t="str">
         <f>_xlfn.IFNA(VLOOKUP(G81,AKUN!A$1:B$1000,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>12</v>
       </c>
@@ -2076,7 +2086,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>AKUN!$A$1:$A$1000</xm:f>
           </x14:formula1>
@@ -2089,16 +2099,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -2106,7 +2116,7 @@
         <v>1010100</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2114,7 +2124,7 @@
         <v>1010101</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2122,7 +2132,7 @@
         <v>1010102</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2130,7 +2140,7 @@
         <v>1010200</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2138,7 +2148,7 @@
         <v>1010201</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2146,7 +2156,7 @@
         <v>1010202</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2154,7 +2164,7 @@
         <v>1010203</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2162,7 +2172,7 @@
         <v>1010204</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -2170,7 +2180,7 @@
         <v>1010205</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -2178,7 +2188,7 @@
         <v>1010300</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -2186,7 +2196,7 @@
         <v>1010301</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -2194,7 +2204,7 @@
         <v>1010302</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2202,7 +2212,7 @@
         <v>1010303</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2210,7 +2220,7 @@
         <v>1010304</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -2218,7 +2228,7 @@
         <v>1010305</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -2226,7 +2236,7 @@
         <v>1010306</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2234,7 +2244,7 @@
         <v>1010307</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -2242,7 +2252,7 @@
         <v>1010308</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -2250,7 +2260,7 @@
         <v>1010309</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -2258,7 +2268,7 @@
         <v>1010310</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -2266,7 +2276,7 @@
         <v>1010311</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -2274,7 +2284,7 @@
         <v>1010312</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -2282,7 +2292,7 @@
         <v>1010313</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -2290,7 +2300,7 @@
         <v>1020100</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -2298,7 +2308,7 @@
         <v>1020101</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -2306,7 +2316,7 @@
         <v>1020102</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -2314,7 +2324,7 @@
         <v>1020103</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -2322,7 +2332,7 @@
         <v>1020104</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -2330,7 +2340,7 @@
         <v>1020105</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -2338,7 +2348,7 @@
         <v>1020106</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -2346,7 +2356,7 @@
         <v>1020107</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -2354,7 +2364,7 @@
         <v>1020108</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -2362,7 +2372,7 @@
         <v>1020109</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -2370,7 +2380,7 @@
         <v>1030100</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -2378,7 +2388,7 @@
         <v>1030101</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -2386,7 +2396,7 @@
         <v>1030102</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -2394,7 +2404,7 @@
         <v>1030103</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -2402,7 +2412,7 @@
         <v>1030104</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -2410,7 +2420,7 @@
         <v>1030105</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -2418,7 +2428,7 @@
         <v>1030106</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -2426,7 +2436,7 @@
         <v>1040100</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -2434,7 +2444,7 @@
         <v>1040101</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -2442,7 +2452,7 @@
         <v>1040102</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>56</v>
       </c>
@@ -2450,7 +2460,7 @@
         <v>1040103</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>57</v>
       </c>
@@ -2458,7 +2468,7 @@
         <v>1040104</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -2466,7 +2476,7 @@
         <v>1040105</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>59</v>
       </c>
@@ -2474,7 +2484,7 @@
         <v>1040106</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -2482,7 +2492,7 @@
         <v>1040107</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -2490,7 +2500,7 @@
         <v>1040108</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>62</v>
       </c>
@@ -2498,7 +2508,7 @@
         <v>1040109</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -2506,7 +2516,7 @@
         <v>1040110</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>64</v>
       </c>
@@ -2514,7 +2524,7 @@
         <v>1040111</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>65</v>
       </c>
@@ -2522,7 +2532,7 @@
         <v>1040112</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>66</v>
       </c>
@@ -2530,7 +2540,7 @@
         <v>1040113</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>67</v>
       </c>
@@ -2538,7 +2548,7 @@
         <v>1040114</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>68</v>
       </c>
@@ -2546,7 +2556,7 @@
         <v>1050100</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>69</v>
       </c>
@@ -2554,7 +2564,7 @@
         <v>1050101</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -2562,7 +2572,7 @@
         <v>1050102</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>71</v>
       </c>
@@ -2570,7 +2580,7 @@
         <v>1050103</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -2578,7 +2588,7 @@
         <v>1050200</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -2586,7 +2596,7 @@
         <v>1050201</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -2594,7 +2604,7 @@
         <v>1050202</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -2602,7 +2612,7 @@
         <v>1050203</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>76</v>
       </c>
@@ -2610,7 +2620,7 @@
         <v>1110100</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -2618,7 +2628,7 @@
         <v>1110101</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>78</v>
       </c>
@@ -2626,7 +2636,7 @@
         <v>1110201</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -2634,7 +2644,7 @@
         <v>1110301</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>80</v>
       </c>
@@ -2642,7 +2652,7 @@
         <v>1110401</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>81</v>
       </c>
@@ -2650,7 +2660,7 @@
         <v>1120100</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>82</v>
       </c>
@@ -2658,7 +2668,7 @@
         <v>1120201</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>83</v>
       </c>
@@ -2666,7 +2676,7 @@
         <v>1120301</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>84</v>
       </c>
@@ -2674,7 +2684,7 @@
         <v>1120401</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -2682,7 +2692,7 @@
         <v>1130100</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>86</v>
       </c>
@@ -2690,7 +2700,7 @@
         <v>1130101</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>87</v>
       </c>
@@ -2698,7 +2708,7 @@
         <v>1130102</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>88</v>
       </c>
@@ -2706,7 +2716,7 @@
         <v>1140100</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>89</v>
       </c>
@@ -2714,7 +2724,7 @@
         <v>1140101</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>90</v>
       </c>
@@ -2722,7 +2732,7 @@
         <v>1140102</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>91</v>
       </c>
@@ -2730,7 +2740,7 @@
         <v>2010100</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>92</v>
       </c>
@@ -2738,7 +2748,7 @@
         <v>2010101</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>93</v>
       </c>
@@ -2746,7 +2756,7 @@
         <v>2010102</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>94</v>
       </c>
@@ -2754,7 +2764,7 @@
         <v>2010103</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>95</v>
       </c>
@@ -2762,7 +2772,7 @@
         <v>2010104</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>96</v>
       </c>
@@ -2770,7 +2780,7 @@
         <v>2010105</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>97</v>
       </c>
@@ -2778,7 +2788,7 @@
         <v>2010106</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>98</v>
       </c>
@@ -2786,7 +2796,7 @@
         <v>2010200</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>99</v>
       </c>
@@ -2794,7 +2804,7 @@
         <v>2010201</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>100</v>
       </c>
@@ -2802,7 +2812,7 @@
         <v>2010202</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>101</v>
       </c>
@@ -2810,7 +2820,7 @@
         <v>2010203</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>102</v>
       </c>
@@ -2818,7 +2828,7 @@
         <v>2010204</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>103</v>
       </c>
@@ -2826,7 +2836,7 @@
         <v>2020100</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>104</v>
       </c>
@@ -2834,7 +2844,7 @@
         <v>2020101</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>105</v>
       </c>
@@ -2842,7 +2852,7 @@
         <v>2020201</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>106</v>
       </c>
@@ -2850,7 +2860,7 @@
         <v>2030100</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>107</v>
       </c>
@@ -2858,7 +2868,7 @@
         <v>2030101</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>108</v>
       </c>
@@ -2866,7 +2876,7 @@
         <v>2030102</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>109</v>
       </c>
@@ -2874,7 +2884,7 @@
         <v>2030103</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>110</v>
       </c>
@@ -2882,7 +2892,7 @@
         <v>2030104</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>111</v>
       </c>
@@ -2890,7 +2900,7 @@
         <v>2030105</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>112</v>
       </c>
@@ -2898,7 +2908,7 @@
         <v>2030106</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>113</v>
       </c>
@@ -2906,7 +2916,7 @@
         <v>2030107</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>114</v>
       </c>
@@ -2914,7 +2924,7 @@
         <v>2030108</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>115</v>
       </c>
@@ -2922,7 +2932,7 @@
         <v>2030109</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>116</v>
       </c>
@@ -2930,7 +2940,7 @@
         <v>2030110</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>117</v>
       </c>
@@ -2938,7 +2948,7 @@
         <v>2030111</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>118</v>
       </c>
@@ -2946,7 +2956,7 @@
         <v>3010100</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>119</v>
       </c>
@@ -2954,7 +2964,7 @@
         <v>3010101</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>120</v>
       </c>
@@ -2962,7 +2972,7 @@
         <v>3010102</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>121</v>
       </c>
@@ -2970,7 +2980,7 @@
         <v>3010103</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>122</v>
       </c>
@@ -2978,7 +2988,7 @@
         <v>3020100</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>123</v>
       </c>
@@ -2986,7 +2996,7 @@
         <v>3020101</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>124</v>
       </c>
@@ -2994,7 +3004,7 @@
         <v>3020102</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>125</v>
       </c>
@@ -3002,7 +3012,7 @@
         <v>4010100</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>126</v>
       </c>
@@ -3010,7 +3020,7 @@
         <v>4010101</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>127</v>
       </c>
@@ -3018,7 +3028,7 @@
         <v>4010102</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>128</v>
       </c>
@@ -3026,7 +3036,7 @@
         <v>4010103</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>129</v>
       </c>
@@ -3034,7 +3044,7 @@
         <v>4010104</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>130</v>
       </c>
@@ -3042,7 +3052,7 @@
         <v>4010200</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>131</v>
       </c>
@@ -3050,7 +3060,7 @@
         <v>4010201</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>132</v>
       </c>
@@ -3058,7 +3068,7 @@
         <v>4010202</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>133</v>
       </c>
@@ -3066,7 +3076,7 @@
         <v>4010203</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>134</v>
       </c>
@@ -3074,7 +3084,7 @@
         <v>4010204</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>135</v>
       </c>
@@ -3082,7 +3092,7 @@
         <v>4010205</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>136</v>
       </c>
@@ -3090,7 +3100,7 @@
         <v>4010206</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>137</v>
       </c>
@@ -3098,7 +3108,7 @@
         <v>4010207</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>138</v>
       </c>
@@ -3106,7 +3116,7 @@
         <v>4010208</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>139</v>
       </c>
@@ -3114,7 +3124,7 @@
         <v>4010209</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>140</v>
       </c>
@@ -3122,7 +3132,7 @@
         <v>4010300</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>141</v>
       </c>
@@ -3130,7 +3140,7 @@
         <v>4010301</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>142</v>
       </c>
@@ -3138,7 +3148,7 @@
         <v>5010100</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>143</v>
       </c>
@@ -3146,7 +3156,7 @@
         <v>5010101</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>144</v>
       </c>
@@ -3154,7 +3164,7 @@
         <v>5010102</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>145</v>
       </c>
@@ -3162,7 +3172,7 @@
         <v>5010103</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>146</v>
       </c>
@@ -3170,7 +3180,7 @@
         <v>5010104</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>147</v>
       </c>
@@ -3178,7 +3188,7 @@
         <v>5010105</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>148</v>
       </c>
@@ -3186,7 +3196,7 @@
         <v>5010106</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>149</v>
       </c>
@@ -3194,7 +3204,7 @@
         <v>5010107</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>150</v>
       </c>
@@ -3202,7 +3212,7 @@
         <v>5010108</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>151</v>
       </c>
@@ -3210,7 +3220,7 @@
         <v>5010109</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>152</v>
       </c>
@@ -3218,7 +3228,7 @@
         <v>5010110</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>153</v>
       </c>
@@ -3226,7 +3236,7 @@
         <v>5010111</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>154</v>
       </c>
@@ -3234,7 +3244,7 @@
         <v>5010112</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>155</v>
       </c>
@@ -3242,7 +3252,7 @@
         <v>5010113</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>156</v>
       </c>
@@ -3250,7 +3260,7 @@
         <v>5010114</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>157</v>
       </c>
@@ -3258,7 +3268,7 @@
         <v>5020100</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>158</v>
       </c>
@@ -3266,7 +3276,7 @@
         <v>5020101</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>159</v>
       </c>
@@ -3274,7 +3284,7 @@
         <v>5020102</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>160</v>
       </c>
@@ -3282,7 +3292,7 @@
         <v>5020103</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>161</v>
       </c>
@@ -3290,7 +3300,7 @@
         <v>5030100</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>162</v>
       </c>
@@ -3298,7 +3308,7 @@
         <v>5030101</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>163</v>
       </c>
@@ -3306,7 +3316,7 @@
         <v>5030102</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>164</v>
       </c>
@@ -3314,7 +3324,7 @@
         <v>5030103</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>165</v>
       </c>
@@ -3322,7 +3332,7 @@
         <v>5030104</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>166</v>
       </c>
@@ -3330,7 +3340,7 @@
         <v>5030105</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>167</v>
       </c>
@@ -3338,7 +3348,7 @@
         <v>5030106</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>168</v>
       </c>
@@ -3346,7 +3356,7 @@
         <v>5030107</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>169</v>
       </c>
@@ -3354,7 +3364,7 @@
         <v>5030108</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>170</v>
       </c>
@@ -3362,7 +3372,7 @@
         <v>5030109</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>171</v>
       </c>
@@ -3370,7 +3380,7 @@
         <v>5030110</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>172</v>
       </c>
@@ -3378,7 +3388,7 @@
         <v>5030111</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>173</v>
       </c>
@@ -3386,7 +3396,7 @@
         <v>5030112</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>174</v>
       </c>
@@ -3394,7 +3404,7 @@
         <v>5030113</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>175</v>
       </c>
@@ -3402,7 +3412,7 @@
         <v>5030114</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>176</v>
       </c>
@@ -3410,7 +3420,7 @@
         <v>5030115</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>177</v>
       </c>
@@ -3418,7 +3428,7 @@
         <v>5030116</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>178</v>
       </c>
@@ -3426,7 +3436,7 @@
         <v>5030117</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>179</v>
       </c>
@@ -3434,7 +3444,7 @@
         <v>5030118</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>180</v>
       </c>
@@ -3442,7 +3452,7 @@
         <v>5030119</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>181</v>
       </c>
@@ -3450,7 +3460,7 @@
         <v>5030120</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>182</v>
       </c>
@@ -3458,7 +3468,7 @@
         <v>5030121</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>183</v>
       </c>
@@ -3466,7 +3476,7 @@
         <v>5030122</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>178</v>
       </c>
@@ -3474,7 +3484,7 @@
         <v>5030123</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>184</v>
       </c>
@@ -3482,7 +3492,7 @@
         <v>5030124</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>185</v>
       </c>
@@ -3490,7 +3500,7 @@
         <v>5030125</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>186</v>
       </c>
@@ -3498,7 +3508,7 @@
         <v>5030126</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>187</v>
       </c>
@@ -3506,7 +3516,7 @@
         <v>5030127</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>188</v>
       </c>
@@ -3514,7 +3524,7 @@
         <v>5030128</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>189</v>
       </c>
@@ -3522,7 +3532,7 @@
         <v>5030129</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>190</v>
       </c>
@@ -3530,7 +3540,7 @@
         <v>5030130</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>191</v>
       </c>
@@ -3538,7 +3548,7 @@
         <v>5030131</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>192</v>
       </c>
@@ -3546,7 +3556,7 @@
         <v>5030132</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>193</v>
       </c>
@@ -3554,7 +3564,7 @@
         <v>5030133</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>194</v>
       </c>
@@ -3562,7 +3572,7 @@
         <v>5030134</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>195</v>
       </c>
@@ -3570,7 +3580,7 @@
         <v>5030135</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>196</v>
       </c>
@@ -3578,7 +3588,7 @@
         <v>5030136</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>197</v>
       </c>
@@ -3586,7 +3596,7 @@
         <v>5030137</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>198</v>
       </c>
@@ -3594,7 +3604,7 @@
         <v>5030138</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>199</v>
       </c>
@@ -3602,7 +3612,7 @@
         <v>5030139</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>200</v>
       </c>
@@ -3610,7 +3620,7 @@
         <v>5040100</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>201</v>
       </c>
@@ -3618,7 +3628,7 @@
         <v>5040101</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>202</v>
       </c>
@@ -3626,7 +3636,7 @@
         <v>5040102</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>203</v>
       </c>
@@ -3634,7 +3644,7 @@
         <v>5050100</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>204</v>
       </c>
@@ -3642,7 +3652,7 @@
         <v>5050101</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>205</v>
       </c>
@@ -3650,7 +3660,7 @@
         <v>5050102</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>206</v>
       </c>
@@ -3658,7 +3668,7 @@
         <v>5060100</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>207</v>
       </c>
@@ -3666,7 +3676,7 @@
         <v>5060101</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>208</v>
       </c>
@@ -3674,7 +3684,7 @@
         <v>5060102</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>209</v>
       </c>
@@ -3682,7 +3692,7 @@
         <v>5060103</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>210</v>
       </c>
@@ -3690,7 +3700,7 @@
         <v>5060104</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>211</v>
       </c>
@@ -3698,7 +3708,7 @@
         <v>5070100</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>212</v>
       </c>
@@ -3706,7 +3716,7 @@
         <v>5070101</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>213</v>
       </c>
@@ -3714,7 +3724,7 @@
         <v>5070102</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>214</v>
       </c>
@@ -3722,7 +3732,7 @@
         <v>5070103</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>215</v>
       </c>
@@ -3730,7 +3740,7 @@
         <v>5080100</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>216</v>
       </c>

</xml_diff>